<commit_message>
Minor correction on the dummy data: 1. Add class "Awan" in the land dist matrix 2. compile_lcArea as xlsx format
</commit_message>
<xml_diff>
--- a/data_dir/provinces/Jambi/LAND_DIST_MATRIX.xlsx
+++ b/data_dir/provinces/Jambi/LAND_DIST_MATRIX.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PPRK\database\indonesia\provinces\jambi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PPRK\process\projects\2019_07\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F065E265-7374-4A87-BFC2-61E946121570}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC37DEE-83EE-48B7-B242-56F2ABA081E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{8043E039-6114-4397-AC5A-36580B898A8D}"/>
   </bookViews>
@@ -212,7 +212,7 @@
     <t>Kegiatan lainnya</t>
   </si>
   <si>
-    <t>TOTAL</t>
+    <t>Awan</t>
   </si>
 </sst>
 </file>
@@ -580,13 +580,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09FFC2A3-54DD-4439-A94E-E59A7B7809CC}">
-  <dimension ref="A1:X39"/>
+  <dimension ref="A1:Y37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B40" sqref="B40"/>
+      <selection pane="bottomRight" activeCell="Y38" sqref="Y38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -606,968 +606,1013 @@
     <col min="20" max="20" width="12.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="C1">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="D1">
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R1" t="s">
+        <v>52</v>
+      </c>
+      <c r="S1" t="s">
+        <v>53</v>
+      </c>
+      <c r="T1" t="s">
+        <v>54</v>
+      </c>
+      <c r="U1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V1" t="s">
+        <v>56</v>
+      </c>
+      <c r="W1" t="s">
+        <v>57</v>
+      </c>
+      <c r="X1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="E1">
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="F1">
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="G1">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0.1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0.2</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0.3</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="H1">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0.5</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="I1">
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0.2</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="J1">
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0.3</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0.2</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="K1">
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0.3</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="L1">
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0.4</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0.1</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0.9</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0.3</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="M1">
+      <c r="C10">
+        <v>0.1</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0.1</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0.1</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="N1">
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0.2</v>
+      </c>
+      <c r="W11">
+        <v>0.2</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="O1">
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>0.25</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="P1">
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0.25</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>14</v>
-      </c>
-      <c r="Q1">
-        <v>15</v>
-      </c>
-      <c r="R1">
-        <v>16</v>
-      </c>
-      <c r="S1">
-        <v>17</v>
-      </c>
-      <c r="T1">
-        <v>18</v>
-      </c>
-      <c r="U1">
-        <v>19</v>
-      </c>
-      <c r="V1">
-        <v>20</v>
-      </c>
-      <c r="W1">
-        <v>21</v>
-      </c>
-      <c r="X1">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I2" t="s">
-        <v>43</v>
-      </c>
-      <c r="J2" t="s">
-        <v>44</v>
-      </c>
-      <c r="K2" t="s">
-        <v>45</v>
-      </c>
-      <c r="L2" t="s">
-        <v>46</v>
-      </c>
-      <c r="M2" t="s">
-        <v>47</v>
-      </c>
-      <c r="N2" t="s">
-        <v>48</v>
-      </c>
-      <c r="O2" t="s">
-        <v>49</v>
-      </c>
-      <c r="P2" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>51</v>
-      </c>
-      <c r="R2" t="s">
-        <v>52</v>
-      </c>
-      <c r="S2" t="s">
-        <v>53</v>
-      </c>
-      <c r="T2" t="s">
-        <v>54</v>
-      </c>
-      <c r="U2" t="s">
-        <v>55</v>
-      </c>
-      <c r="V2" t="s">
-        <v>56</v>
-      </c>
-      <c r="W2" t="s">
-        <v>57</v>
-      </c>
-      <c r="X2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3">
-        <v>0.9</v>
-      </c>
-      <c r="D3">
-        <v>0.6</v>
-      </c>
-      <c r="E3">
-        <v>0.9</v>
-      </c>
-      <c r="F3">
-        <v>0.9</v>
-      </c>
-      <c r="G3">
-        <v>0.9</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>0.7</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>1</v>
-      </c>
-      <c r="T3">
-        <v>0</v>
-      </c>
-      <c r="U3">
-        <v>0.8</v>
-      </c>
-      <c r="V3">
-        <v>0.8</v>
-      </c>
-      <c r="W3">
-        <v>0.8</v>
-      </c>
-      <c r="X3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>1</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
-      <c r="V4">
-        <v>0</v>
-      </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="X4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="V5">
-        <v>0</v>
-      </c>
-      <c r="W5">
-        <v>0</v>
-      </c>
-      <c r="X5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0.1</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0.2</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>0.3</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-      <c r="V6">
-        <v>0</v>
-      </c>
-      <c r="W6">
-        <v>0</v>
-      </c>
-      <c r="X6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>0.5</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="T7">
-        <v>0</v>
-      </c>
-      <c r="U7">
-        <v>0</v>
-      </c>
-      <c r="V7">
-        <v>0</v>
-      </c>
-      <c r="W7">
-        <v>0</v>
-      </c>
-      <c r="X7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>0.2</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>0</v>
-      </c>
-      <c r="U8">
-        <v>0</v>
-      </c>
-      <c r="V8">
-        <v>0</v>
-      </c>
-      <c r="W8">
-        <v>0</v>
-      </c>
-      <c r="X8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>0.3</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>0.2</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
-      <c r="T9">
-        <v>0</v>
-      </c>
-      <c r="U9">
-        <v>0</v>
-      </c>
-      <c r="V9">
-        <v>0</v>
-      </c>
-      <c r="W9">
-        <v>0</v>
-      </c>
-      <c r="X9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0.3</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-      <c r="R10">
-        <v>0</v>
-      </c>
-      <c r="S10">
-        <v>0</v>
-      </c>
-      <c r="T10">
-        <v>0</v>
-      </c>
-      <c r="U10">
-        <v>0</v>
-      </c>
-      <c r="V10">
-        <v>0</v>
-      </c>
-      <c r="W10">
-        <v>0</v>
-      </c>
-      <c r="X10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0.4</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0.1</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0.9</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <v>0.3</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-      <c r="R11">
-        <v>0</v>
-      </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
-      <c r="T11">
-        <v>0</v>
-      </c>
-      <c r="U11">
-        <v>0</v>
-      </c>
-      <c r="V11">
-        <v>0</v>
-      </c>
-      <c r="W11">
-        <v>0</v>
-      </c>
-      <c r="X11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12">
-        <v>0.1</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0.1</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0.1</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12">
-        <v>0</v>
-      </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
-      <c r="R12">
-        <v>0</v>
-      </c>
-      <c r="S12">
-        <v>0</v>
-      </c>
-      <c r="T12">
-        <v>0</v>
-      </c>
-      <c r="U12">
-        <v>0</v>
-      </c>
-      <c r="V12">
-        <v>0</v>
-      </c>
-      <c r="W12">
-        <v>0</v>
-      </c>
-      <c r="X12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
-      <c r="Q13">
-        <v>0</v>
-      </c>
-      <c r="R13">
-        <v>1</v>
-      </c>
-      <c r="S13">
-        <v>0</v>
-      </c>
-      <c r="T13">
-        <v>0</v>
-      </c>
-      <c r="U13">
-        <v>0</v>
-      </c>
-      <c r="V13">
-        <v>0.2</v>
-      </c>
-      <c r="W13">
-        <v>0.2</v>
-      </c>
-      <c r="X13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>11</v>
-      </c>
-      <c r="B14" t="s">
-        <v>12</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1635,13 +1680,16 @@
       <c r="X14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1709,13 +1757,16 @@
       <c r="X15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1769,10 +1820,10 @@
         <v>0</v>
       </c>
       <c r="T16">
-        <v>0.25</v>
-      </c>
-      <c r="U16">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="U16" s="1">
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="V16">
         <v>0</v>
@@ -1783,13 +1834,16 @@
       <c r="X16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1843,10 +1897,10 @@
         <v>0</v>
       </c>
       <c r="T17">
-        <v>0.25</v>
-      </c>
-      <c r="U17">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="U17" s="1">
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="V17">
         <v>0</v>
@@ -1857,13 +1911,16 @@
       <c r="X17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1931,13 +1988,16 @@
       <c r="X18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -2005,13 +2065,16 @@
       <c r="X19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -2079,13 +2142,16 @@
       <c r="X20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -2153,13 +2219,16 @@
       <c r="X21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -2227,13 +2296,16 @@
       <c r="X22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -2301,13 +2373,16 @@
       <c r="X23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -2375,13 +2450,16 @@
       <c r="X24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -2449,13 +2527,16 @@
       <c r="X25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -2511,8 +2592,8 @@
       <c r="T26">
         <v>0</v>
       </c>
-      <c r="U26" s="1">
-        <v>1.4999999999999999E-2</v>
+      <c r="U26">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="V26">
         <v>0</v>
@@ -2523,13 +2604,16 @@
       <c r="X26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -2585,8 +2669,8 @@
       <c r="T27">
         <v>0</v>
       </c>
-      <c r="U27" s="1">
-        <v>1.4999999999999999E-2</v>
+      <c r="U27">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="V27">
         <v>0</v>
@@ -2597,13 +2681,16 @@
       <c r="X27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -2660,7 +2747,7 @@
         <v>0</v>
       </c>
       <c r="U28">
-        <v>5.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="V28">
         <v>0</v>
@@ -2669,15 +2756,18 @@
         <v>0</v>
       </c>
       <c r="X28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="Y28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -2745,13 +2835,16 @@
       <c r="X29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -2808,7 +2901,7 @@
         <v>0</v>
       </c>
       <c r="U30">
-        <v>0</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="V30">
         <v>0</v>
@@ -2817,15 +2910,18 @@
         <v>0</v>
       </c>
       <c r="X30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="Y30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -2893,13 +2989,16 @@
       <c r="X31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -2967,13 +3066,16 @@
       <c r="X32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -3041,13 +3143,16 @@
       <c r="X33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -3115,13 +3220,16 @@
       <c r="X34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -3189,13 +3297,16 @@
       <c r="X35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -3263,43 +3374,46 @@
       <c r="X36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="F37">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="G37">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="H37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37">
         <v>0</v>
       </c>
       <c r="J37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L37">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="M37">
         <v>0</v>
@@ -3311,7 +3425,7 @@
         <v>0</v>
       </c>
       <c r="P37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q37">
         <v>0</v>
@@ -3320,188 +3434,24 @@
         <v>0</v>
       </c>
       <c r="S37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T37">
         <v>0</v>
       </c>
       <c r="U37">
-        <v>5.0000000000000001E-3</v>
+        <v>0.8</v>
       </c>
       <c r="V37">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="W37">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="X37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A38">
-        <v>35</v>
-      </c>
-      <c r="B38" t="s">
-        <v>36</v>
-      </c>
-      <c r="C38">
-        <v>0</v>
-      </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
-      <c r="E38">
-        <v>0</v>
-      </c>
-      <c r="F38">
-        <v>0</v>
-      </c>
-      <c r="G38">
-        <v>0</v>
-      </c>
-      <c r="H38">
-        <v>0</v>
-      </c>
-      <c r="I38">
-        <v>0</v>
-      </c>
-      <c r="J38">
-        <v>0</v>
-      </c>
-      <c r="K38">
-        <v>0</v>
-      </c>
-      <c r="L38">
-        <v>0</v>
-      </c>
-      <c r="M38">
-        <v>0</v>
-      </c>
-      <c r="N38">
-        <v>0</v>
-      </c>
-      <c r="O38">
-        <v>0</v>
-      </c>
-      <c r="P38">
-        <v>0</v>
-      </c>
-      <c r="Q38">
-        <v>0</v>
-      </c>
-      <c r="R38">
-        <v>0</v>
-      </c>
-      <c r="S38">
-        <v>0</v>
-      </c>
-      <c r="T38">
-        <v>0</v>
-      </c>
-      <c r="U38">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="V38">
-        <v>0</v>
-      </c>
-      <c r="W38">
-        <v>0</v>
-      </c>
-      <c r="X38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="B39" t="s">
-        <v>60</v>
-      </c>
-      <c r="C39">
-        <f>SUM(C3:C38)</f>
-        <v>1</v>
-      </c>
-      <c r="D39">
-        <f t="shared" ref="D39:X39" si="0">SUM(D3:D38)</f>
-        <v>1</v>
-      </c>
-      <c r="E39">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F39">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G39">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H39">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I39">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J39">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K39">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="L39">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M39">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="N39">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="O39">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="P39">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="Q39">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="R39">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="S39">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="T39">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="U39">
-        <f t="shared" si="0"/>
-        <v>1.0000000000000002</v>
-      </c>
-      <c r="V39">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="W39">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="X39">
-        <f t="shared" si="0"/>
+      <c r="Y37">
         <v>1</v>
       </c>
     </row>

</xml_diff>